<commit_message>
Small KiCAD footprint update. New DB items. Corrected KiCAD BOM generator multiplier bug.
</commit_message>
<xml_diff>
--- a/pending_DB_additions.xlsx
+++ b/pending_DB_additions.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="809">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -2375,6 +2375,9 @@
     <t xml:space="preserve">SOLDER PASTE WATER SOL LF 10CC</t>
   </si>
   <si>
+    <t xml:space="preserve">material, soldering</t>
+  </si>
+  <si>
     <t xml:space="preserve">SMD4300SNL10T4</t>
   </si>
   <si>
@@ -2385,6 +2388,69 @@
   </si>
   <si>
     <t xml:space="preserve">SINGLE 10-MHZ, 40-V RAIL-TO-RAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTAK04010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAPTON INSULATED CU WIRE,3KV,2A,0.40MM,10M LG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wire, material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accu-Glass Products Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapton UHV Wire, solid, 30AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapton UHV Wire, 7 strand 20WAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harbour Industries Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIL-W-81381/7-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapton Wire, 22AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allied Wire and Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M81381/7-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapton Wire, 24AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha Wire Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2844/19 BK005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24AWG 19/36 TFE stranded wire MIL-W-168780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2854/1 BK005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24AWG TFE solid wire AWM 1213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPI (Test Products Int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD291-10M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REL0 NO-CLEAN FLUX W/ TIPS</t>
   </si>
 </sst>
 </file>
@@ -2395,7 +2461,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2474,6 +2540,18 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -2560,7 +2638,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2633,6 +2711,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2645,7 +2731,7 @@
     <cellStyle name="Excel Built-in Neutral" xfId="21"/>
     <cellStyle name="Excel Built-in Bad" xfId="22"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2693,6 +2779,20 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF0563C1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFCC0000"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2783,12 +2883,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AML354"/>
+  <dimension ref="A1:AML372"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A329" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D347" activeCellId="0" sqref="D347"/>
+      <selection pane="bottomLeft" activeCell="G354" activeCellId="0" sqref="G354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8891,6 +8991,9 @@
       <c r="E352" s="1" t="s">
         <v>782</v>
       </c>
+      <c r="G352" s="1" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="1" t="n">
@@ -8900,10 +9003,13 @@
         <v>780</v>
       </c>
       <c r="D353" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E353" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="G353" s="1" t="s">
         <v>783</v>
-      </c>
-      <c r="E353" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8914,16 +9020,187 @@
         <v>281</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>786</v>
-      </c>
+        <v>787</v>
+      </c>
+      <c r="G354" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="E355" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="G355" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="0" t="n">
+        <v>360</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D356" s="1" t="n">
+        <v>100670</v>
+      </c>
+      <c r="E356" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="G356" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="n">
+        <v>361</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D357" s="1" t="n">
+        <v>112716</v>
+      </c>
+      <c r="E357" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="G357" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="n">
+        <v>362</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="G358" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="n">
+        <v>363</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="E359" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="G359" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="n">
+        <v>364</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E360" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="G360" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A361" s="0" t="n">
+        <v>365</v>
+      </c>
+      <c r="C361" s="0" t="s">
+        <v>801</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="E361" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="G361" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="n">
+        <v>366</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="E362" s="18" t="s">
+        <v>675</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="n">
+        <v>367</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G363" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D369" s="19"/>
+    </row>
+    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D370" s="19"/>
+    </row>
+    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D371" s="19"/>
+    </row>
+    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D372" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I354"/>
-  <conditionalFormatting sqref="D1:D241 D243:D244 D246:D259 D261:D265 D267:D270 D272 D274:D276 D278:D279 D348:D1048576 D281:D295 E296 D297:D300 D302:D346 E347">
+  <conditionalFormatting sqref="D1:D241 D243:D244 D246:D259 D261:D265 D267:D270 D272 D274:D276 D278:D279 D281:D295 E296 D297:D300 D302:D346 E347 D348:D360 D364:D1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D369:D372">
+    <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
General database and CAD data additions. Added quantity distinctions to KiCAD BOM generator.
</commit_message>
<xml_diff>
--- a/pending_DB_additions.xlsx
+++ b/pending_DB_additions.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="1107">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -1628,6 +1628,15 @@
     <t xml:space="preserve">3.5-V TO 80-V, CURRENT MODE SYNC</t>
   </si>
   <si>
+    <t xml:space="preserve">Smiths Interconnect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS-30-B-1.3-G D/C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact Probes 30 DEG SPEAR POINT </t>
+  </si>
+  <si>
     <t xml:space="preserve">LM25148QRGYRQ1</t>
   </si>
   <si>
@@ -2451,6 +2460,891 @@
   </si>
   <si>
     <t xml:space="preserve">REL0 NO-CLEAN FLUX W/ TIPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE MAT RUBBER BLUE 3' X 2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environment, material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE MAT VINYL DARK BLU 4' X 2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE MAT RUBBER BLUE 4' X 2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">415-0029-M1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBL ASSY SMA PLUG TO PLUG 4.9'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">415-0029-M2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBL ASSY SMA PLUG TO PLUG 6.6'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M13146 SL005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTI-PAIR 12COND 20AWG 100'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8700 010250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Audio, #28 TC coax, BC Braid, PVC Jacket, CMH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTC-50-1-1, 0.5Lz/1.5, CEH50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coaxial and Triaxial FRNC-High Voltage Low Power Cables acc. To CERN and DESY Specifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nidec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8A1011-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWITCH TOGGLE SPDT 6A 125V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">part number from part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATSAMA5D27-SOM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC MOD CORTEX-A5 500MHZ 1GB 64MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seeed Studio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wio Terminal: ATSAMD51 Core with Realtek RTL8720DN BLE 5.0 &amp; Wi-Fi 2.4G/5G Dev Board with Free Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAB Embedded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAB-002002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINUX COMPUTE MODULE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adafruit Industries LLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAPT TERM BL 2POS TO 2.1MM JCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adapter, interconnect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCC28C50DGKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDUSTRIAL, 30-V, LOW-POWER CURR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS90CP02SP/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CROSSPOINT SW 1 X 2:2 28WQFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCAN90CP02SP/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS15BA101SDE/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REDRIVER LVDS 1CH 8WSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN65LVDS19DRFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REDRIVER 1CH 2GBPS 8WSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS15BR400TSQ/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REDRIVER LVDS 4CH 32WQFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DS90LT012ATMF/NOPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC RECEIVER 0/1 SOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wakefield Vette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SILICONE GREASE 2 OZ JAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material, thermal, chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apex Tool Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XN100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNIFE PRECISION WITH BLADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hand tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XN200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aven Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNIFE PRECISION WITH #11 BLADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNIFE PRECISION WITH #22 BLADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XNB103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPLCMT BLADE KNIFE FINE POINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consumable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XNB205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPLACEMENT BLADE KNIFE POINTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olfa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB-50B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9mm Snap-Off Silver Blade, 50-Pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADP7142ARDZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG LIN POS ADJ 200MA 8SOIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT3082EDD#TRPBF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG LINEAR POS ADJ 200MA 8DFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5PB1108CMGI8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CLK BUFFER 1:8 200MHZ 16QFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LXC1T14DCKR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC TRANSLATOR UNIDIR SC70-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPKF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protomat PCB prototyping mill and vacuum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipment, manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protoflow E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reflow oven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WR3M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combo station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soldering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering power supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC201P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24V 42W soldering Iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603546-I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modu IV 20-32AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crimping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90345-1-E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30-20 Type-F Crimper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18-24AWG Type F crimper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63811-1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General purpose service grade crimping tool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90191-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26-32 Type F Crimper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETP tip for EC2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST4 tip for WP25/WP40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WESD51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PES51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0054444099N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering tip LT A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0054440699</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIP SOLDER CONICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ungar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering tip for 9000 series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DST4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desoldering tip for DS40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WS991-5M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WATER-SOLUBLE TACK FLUX W/TIPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity Passive Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPF0805B8R2E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 8.2 OHM 0.1% 1/10W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMT, resistor, passive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV9062SIRUGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CMOS 2 CIRCUIT 10X2QFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INA180A1IDBVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CURR SENSE 1 CIRCUIT SOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPF0603B8R2E1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES SMD 8.2 OHM 0.1% 1/16W 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD48K25G-TL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC SUPERVISOR 1 CHANNEL 3SSOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-H2GJ1R5X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 1.5 OHM 5% 1/10W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEV-13672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMD21 DEV BREAKOUT EVAL BRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">module, MCU, breakout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATSAMD21G18A-MUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC MCU 32BIT 256KB FLASH 48QFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, MCU, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC-135 32.7680K-60AA70KD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRYSTAL 32.7680KHZ 6PF SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crystal, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC-135 32.7680KF-AG0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRYSTAL 32.7680KHZ 7PF SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NFM15PC474R0J3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP FEEDTHRU 0.47UF 6.3V 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passive, capacitor, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-2BQJR39X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES 0.39 OHM 5% 1/6W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS43TR16640C-125JBL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC DRAM 1GBIT PARALLEL 96TWBGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMT, IC, memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LFE5U-45F-6BG256C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC FPGA 197 I/O 256CABGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, FPGA, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCIMX6Y0CVM05AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC MPU I.MX6 528MHZ 289MAPBGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, MPU, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPC4078FET208K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC MCU 32BIT 512KB FLSH 208TFBGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPC804M101JHI33Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC MCU 32BIT 32KB FLASH 32HVQFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KVR16N11/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingston ValueRAM 8GB 240-Pin PC RAM DDR3 1600 (PC3 12800) Desktop Memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">module, memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monolithic Power Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP3217DJ-LF-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG BOOST ADJ 500MA TSOT23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, SMT, regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MP3209DJ-LF-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG BOOST ADJ 350MA TSOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP3015KTR-G1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG BOOST ADJ 300MA SOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGM05AR71E104KH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.1UF 25V X7R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB4145-03-0230-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB 2.0 TYPE-C RECPT VERT SMT 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, connector, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2N7002-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET N-CH 60V 115MA SOT23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transistor, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI3L2500ZHEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC LAN SWITCH V-QFN3590-42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, SMT, switch, analog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74AVC4T3144GU12-QX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC TRANSLATOR UNIDIR 12XQFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, SMT, logic, digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74LVC1G08GM,132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC GATE AND 1CH 2-INP 6XSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3223W-1-103E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIMMER 10KOHM 0.125W J LEAD TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passive, electromechanical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LMG1020YFFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC GATE DRVR LOW-SIDE 6DSBGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMEG4030ER,115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIODE SCHOTTKY 40V 3A SOD123W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">discrete, diode, SMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADP7142AUJZ-R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG LIN POS ADJ 200MA TSOT23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KGA05AS70J104MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.1UF 6.3V X7S 0204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0510X7R1E473M030BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMMERCIAL GRADE REVERSE GEOMETR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5PB1102CMGI8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CLOCK BUFFER 1:2 8DFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC, SMT, digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN SMA JACK STR 50 OHM PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMA JACK VERTICAL PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlobTek Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23214272M5701(R)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORD 17AWG SEV 3 POS-IEC320 8.2'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, cable, power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIRCUIT BRAKER 10A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safety, power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altech Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUE325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOTOR DISCONNECT SWITCH 3P TOGGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power, electromechanical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schurter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PWR ENT RCPT IEC320-C14 PANEL QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hammond Manufacturing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1590K432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOX ZINC UNPTD 7.402"L X 4.724"W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enclosure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOX STEEL GRAY 8"L X 8"W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSKO884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHKO884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOX STEEL GRAY 8"L X 6"W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hubbell Wiring Device-Kellems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UFC0003CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cord Connectors, Underground Feeder Connectors, .2"x.6" min, .26"x.78" max, 3/4", Nylon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power, marine, grommet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABB T&amp;B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAB2520</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABB 1/2 inch, .125-.250 range, T&amp;B Liquidtight Strain Relief Cord Connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grommet, accessory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hubbel Raco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4804-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRAIN RELIEF CONDUIT AND CORD CONNECTORS - ALUMINUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2922AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cable Gland, Strain Relief, Straight, 1/2" NPT, 0.5 ", 0.75 ", Aluminum, Metallic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heyco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG 50A-250 (RED GLAND)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1546306-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN BARRIER STRIP 5CIRC 0.374"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power, interconnect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1776293-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN TERM STRIP 5CIRC 0.315"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN74LVTH125RGYR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC BUF NON-INVERT 3.6V 14VQFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN BNC JACK STR 50 OHM CRIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, connector, coaxial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lumex Opto/Components Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSI-LXH312GD-150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED 3MM GREEN 6"LDS PANEL MOUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optoelectronics, photonics, diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">198-170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS35-170 DIN RAIL FOR TG2015 ENC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2110A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel Mount Indicator Lamps RED DIFFUSED 5/16" MOUNTING HOLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">optoelectronics, photonics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10114828-10108LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HEADER SMD 8POS 1.25MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10114826-00008LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN RCPT HSG 8POS 1.25MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, connector, housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-747909-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN D-SUB RCPT 15POS SLDR CUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, backshell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5206471-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN BACKSHELL 15P 180DEG GRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5745172-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN BACKSHELL 15POS 180DEG SHLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">205205-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN D-SUB HOUSING RCPT 15POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166051-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN D-SUB SOCKET 20-24AWG CRIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66504-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN SOCKET 20-24AWG GOLD CRIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66504-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tripp Lite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N033-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN MOD COUPLER 8P8C TO 8P8C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interconnect, coupler</t>
   </si>
 </sst>
 </file>
@@ -2547,6 +3441,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2883,12 +3778,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AML372"/>
+  <dimension ref="A1:AML483"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G354" activeCellId="0" sqref="G354"/>
+      <selection pane="bottomLeft" activeCell="G484" activeCellId="0" sqref="G484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7309,6 +8204,15 @@
       <c r="A242" s="1" t="n">
         <v>246</v>
       </c>
+      <c r="C242" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
@@ -7318,10 +8222,10 @@
         <v>281</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7332,10 +8236,10 @@
         <v>281</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7346,10 +8250,10 @@
         <v>281</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="G245" s="1" t="s">
         <v>420</v>
@@ -7360,13 +8264,13 @@
         <v>250</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="G246" s="1" t="s">
         <v>420</v>
@@ -7377,13 +8281,13 @@
         <v>251</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="D247" s="1" t="n">
         <v>40852</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="G247" s="1" t="s">
         <v>420</v>
@@ -7394,13 +8298,13 @@
         <v>252</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="G248" s="1" t="s">
         <v>420</v>
@@ -7414,10 +8318,10 @@
         <v>414</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="G249" s="1" t="s">
         <v>420</v>
@@ -7431,10 +8335,10 @@
         <v>414</v>
       </c>
       <c r="D250" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>544</v>
       </c>
       <c r="G250" s="1" t="s">
         <v>420</v>
@@ -7445,10 +8349,10 @@
         <v>255</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>464</v>
@@ -7465,10 +8369,10 @@
         <v>207</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="G252" s="1" t="s">
         <v>420</v>
@@ -7482,10 +8386,10 @@
         <v>207</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="G253" s="1" t="s">
         <v>420</v>
@@ -7499,10 +8403,10 @@
         <v>207</v>
       </c>
       <c r="D254" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E254" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="E254" s="1" t="s">
-        <v>551</v>
       </c>
       <c r="G254" s="1" t="s">
         <v>420</v>
@@ -7516,7 +8420,7 @@
         <v>207</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>464</v>
@@ -7530,10 +8434,10 @@
         <v>260</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E256" s="1" t="s">
         <v>464</v>
@@ -7547,13 +8451,13 @@
         <v>261</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="G257" s="1" t="s">
         <v>420</v>
@@ -7564,13 +8468,13 @@
         <v>262</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7581,10 +8485,10 @@
         <v>207</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="G259" s="1" t="s">
         <v>420</v>
@@ -7598,10 +8502,10 @@
         <v>207</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="G260" s="1" t="s">
         <v>420</v>
@@ -7612,13 +8516,13 @@
         <v>265</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7626,13 +8530,13 @@
         <v>266</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7643,10 +8547,10 @@
         <v>281</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="G263" s="1" t="s">
         <v>420</v>
@@ -7660,10 +8564,10 @@
         <v>442</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="G264" s="1" t="s">
         <v>420</v>
@@ -7677,10 +8581,10 @@
         <v>414</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="G265" s="1" t="s">
         <v>420</v>
@@ -7694,10 +8598,10 @@
         <v>442</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="G266" s="1" t="s">
         <v>420</v>
@@ -7708,13 +8612,13 @@
         <v>271</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="G267" s="1" t="s">
         <v>420</v>
@@ -7728,10 +8632,10 @@
         <v>428</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="G268" s="1" t="s">
         <v>420</v>
@@ -7742,13 +8646,13 @@
         <v>273</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="G269" s="1" t="s">
         <v>420</v>
@@ -7759,19 +8663,19 @@
         <v>274</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="G270" s="1" t="s">
         <v>420</v>
       </c>
       <c r="H270" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7779,13 +8683,13 @@
         <v>275</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="G271" s="1" t="s">
         <v>420</v>
@@ -7799,10 +8703,10 @@
         <v>237</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7816,7 +8720,7 @@
         <v>530</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="G273" s="1" t="s">
         <v>420</v>
@@ -7827,13 +8731,13 @@
         <v>278</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7841,13 +8745,13 @@
         <v>279</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7855,13 +8759,13 @@
         <v>280</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7875,7 +8779,7 @@
         <v>654</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7883,13 +8787,13 @@
         <v>282</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7897,13 +8801,13 @@
         <v>283</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7925,10 +8829,10 @@
         <v>237</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7936,13 +8840,13 @@
         <v>286</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="G282" s="1" t="s">
         <v>420</v>
@@ -7956,10 +8860,10 @@
         <v>422</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7970,10 +8874,10 @@
         <v>121</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7981,13 +8885,13 @@
         <v>289</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7995,13 +8899,13 @@
         <v>290</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8012,10 +8916,10 @@
         <v>205</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8026,10 +8930,10 @@
         <v>121</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8040,10 +8944,10 @@
         <v>121</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8051,13 +8955,13 @@
         <v>294</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8065,13 +8969,13 @@
         <v>295</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="D291" s="1" t="n">
         <v>102110420</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8079,13 +8983,13 @@
         <v>296</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8093,13 +8997,13 @@
         <v>297</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="D293" s="1" t="n">
         <v>104067</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="G293" s="1" t="s">
         <v>82</v>
@@ -8110,13 +9014,13 @@
         <v>298</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="G294" s="1" t="s">
         <v>82</v>
@@ -8127,13 +9031,13 @@
         <v>299</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8144,13 +9048,13 @@
         <v>207</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8161,13 +9065,13 @@
         <v>207</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8175,16 +9079,16 @@
         <v>302</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8192,13 +9096,13 @@
         <v>303</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8206,13 +9110,13 @@
         <v>304</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8220,16 +9124,16 @@
         <v>305</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8240,10 +9144,10 @@
         <v>414</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8251,13 +9155,13 @@
         <v>307</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="D303" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="E303" s="1" t="s">
         <v>667</v>
-      </c>
-      <c r="E303" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8268,10 +9172,10 @@
         <v>414</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8282,10 +9186,10 @@
         <v>207</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="E305" s="1" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8296,10 +9200,10 @@
         <v>414</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="E306" s="1" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8307,13 +9211,13 @@
         <v>311</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="E307" s="1" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8321,13 +9225,13 @@
         <v>312</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8335,13 +9239,13 @@
         <v>313</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="E309" s="1" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8349,13 +9253,13 @@
         <v>314</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="E310" s="1" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8363,13 +9267,13 @@
         <v>315</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="E311" s="1" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8377,13 +9281,13 @@
         <v>316</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8391,13 +9295,13 @@
         <v>317</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="E313" s="1" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8405,13 +9309,13 @@
         <v>318</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="E314" s="1" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8422,10 +9326,10 @@
         <v>271</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="E315" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8436,10 +9340,10 @@
         <v>271</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="E316" s="1" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8450,10 +9354,10 @@
         <v>271</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="E317" s="1" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8461,13 +9365,13 @@
         <v>322</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="E318" s="1" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8478,10 +9382,10 @@
         <v>121</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="E319" s="1" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8489,16 +9393,16 @@
         <v>324</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8509,13 +9413,13 @@
         <v>281</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
       <c r="E321" s="1" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8526,13 +9430,13 @@
         <v>442</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="E322" s="1" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8543,13 +9447,13 @@
         <v>422</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="E323" s="1" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8560,10 +9464,10 @@
         <v>422</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="E324" s="1" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8571,13 +9475,13 @@
         <v>329</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="E325" s="17" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="F325" s="1"/>
     </row>
@@ -8586,13 +9490,13 @@
         <v>330</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="E326" s="1" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8600,13 +9504,13 @@
         <v>331</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="E327" s="1" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8620,7 +9524,7 @@
         <v>132114</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8628,13 +9532,13 @@
         <v>333</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8642,13 +9546,13 @@
         <v>334</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="D330" s="2" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8659,10 +9563,10 @@
         <v>281</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
       <c r="E331" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8673,10 +9577,10 @@
         <v>281</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
       <c r="E332" s="1" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8684,13 +9588,13 @@
         <v>337</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="E333" s="1" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8698,13 +9602,13 @@
         <v>338</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8718,7 +9622,7 @@
         <v>132170</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8732,7 +9636,7 @@
         <v>150260210</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8743,10 +9647,10 @@
         <v>390</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8757,10 +9661,10 @@
         <v>390</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8771,10 +9675,10 @@
         <v>366</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="G339" s="1" t="s">
         <v>420</v>
@@ -8785,16 +9689,16 @@
         <v>344</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="E340" s="1" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8802,16 +9706,16 @@
         <v>345</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="E341" s="1" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8819,16 +9723,16 @@
         <v>346</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="D342" s="1" t="n">
         <v>515</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8836,13 +9740,13 @@
         <v>347</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="E343" s="1" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8850,16 +9754,16 @@
         <v>348</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
       <c r="E344" s="1" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
       <c r="G344" s="1" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8867,16 +9771,16 @@
         <v>349</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
       <c r="G345" s="1" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8884,16 +9788,16 @@
         <v>350</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
       <c r="D346" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="G346" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="E346" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="G346" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8901,16 +9805,16 @@
         <v>351</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="D347" s="1" t="n">
         <v>550</v>
       </c>
       <c r="E347" s="1" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
       <c r="G347" s="1" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8918,13 +9822,13 @@
         <v>352</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8935,10 +9839,10 @@
         <v>281</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="E349" s="2" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="G349" s="1" t="s">
         <v>420</v>
@@ -8949,16 +9853,16 @@
         <v>354</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="E350" s="1" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8966,16 +9870,16 @@
         <v>355</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="E351" s="1" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8983,16 +9887,16 @@
         <v>356</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9000,16 +9904,16 @@
         <v>357</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>784</v>
+        <v>787</v>
       </c>
       <c r="E353" s="1" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="G353" s="1" t="s">
-        <v>783</v>
+        <v>786</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9020,13 +9924,13 @@
         <v>281</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9034,172 +9938,2185 @@
         <v>359</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="E355" s="1" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="G355" s="1" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="0" t="n">
+      <c r="A356" s="1" t="n">
         <v>360</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="D356" s="1" t="n">
         <v>100670</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="0" t="n">
+      <c r="A357" s="1" t="n">
         <v>361</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="D357" s="1" t="n">
         <v>112716</v>
       </c>
       <c r="E357" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="G357" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="G357" s="1" t="s">
-        <v>791</v>
-      </c>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="0" t="n">
+      <c r="A358" s="1" t="n">
         <v>362</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="G358" s="1" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="0" t="n">
+      <c r="A359" s="1" t="n">
         <v>363</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="E359" s="1" t="s">
-        <v>800</v>
+        <v>803</v>
       </c>
       <c r="G359" s="1" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="0" t="n">
+      <c r="A360" s="1" t="n">
         <v>364</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="E360" s="1" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="G360" s="1" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="0" t="n">
+      <c r="A361" s="1" t="n">
         <v>365</v>
       </c>
-      <c r="C361" s="0" t="s">
-        <v>801</v>
+      <c r="C361" s="1" t="s">
+        <v>804</v>
       </c>
       <c r="D361" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="E361" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G361" s="1" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E362" s="18" t="s">
+        <v>678</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="G363" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D364" s="1" t="n">
+        <v>66444</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="G364" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D365" s="1" t="n">
+        <v>65140</v>
+      </c>
+      <c r="E365" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="G365" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D366" s="1" t="n">
+        <v>66212</v>
+      </c>
+      <c r="E366" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G366" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="E367" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="G367" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A368" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="E368" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="G368" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="C369" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="E361" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="G361" s="1" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="0" t="n">
+      <c r="D369" s="19" t="s">
+        <v>822</v>
+      </c>
+      <c r="E369" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="G369" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="D370" s="19" t="s">
+        <v>825</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="G370" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="C371" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D371" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="E373" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D374" s="1" t="n">
+        <v>102991299</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A375" s="1" t="n">
+        <v>379</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="E375" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="D376" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="G376" s="1" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="1" t="n">
+        <v>381</v>
+      </c>
+      <c r="C377" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="E377" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="1" t="n">
+        <v>382</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="E378" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="1" t="n">
+        <v>383</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="E379" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="1" t="n">
+        <v>384</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D380" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D381" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="E381" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="C383" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="E383" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="G384" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="E385" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="G385" s="1" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E386" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D387" s="1" t="n">
+        <v>44012</v>
+      </c>
+      <c r="E387" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="G387" s="1" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D388" s="1" t="n">
+        <v>44013</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="G388" s="1" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="E389" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A390" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="E390" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="G390" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="C391" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="E391" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="E392" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="G392" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A393" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A394" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A395" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="E395" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="G395" s="1" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="F396" s="1"/>
+      <c r="G396" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="C397" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="E397" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="F397" s="1"/>
+      <c r="G397" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D398" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="E398" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A399" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="E399" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="G399" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="E400" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="G400" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="E401" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="G401" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="E402" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="G402" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D403" s="2" t="n">
+        <v>90067</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="G403" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="E404" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="G404" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D405" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="E405" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="F405" s="1"/>
+      <c r="G405" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="E406" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="F406" s="1"/>
+      <c r="G406" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="C407" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D407" s="1" t="n">
+        <v>9010</v>
+      </c>
+      <c r="F407" s="1"/>
+      <c r="G407" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D408" s="1" t="n">
+        <v>335901</v>
+      </c>
+      <c r="E408" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="G408" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D409" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="E410" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="F410" s="1"/>
+      <c r="G410" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D411" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="E412" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="G412" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="C413" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D413" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="E413" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="G413" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="D414" s="1" t="n">
+        <v>9018</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="G414" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D415" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="G415" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="E416" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="G416" s="1" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="C417" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="D417" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="G417" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="G418" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D419" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="G419" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="D420" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="E420" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="G420" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="C421" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D421" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="E421" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="G421" s="1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D422" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="E422" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="G422" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="C423" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="G423" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="E424" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="G424" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D425" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="E425" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="G425" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="E426" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="G426" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="G427" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="1" t="n">
+        <v>332</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="E428" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="G428" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="C429" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E429" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="G429" s="1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D430" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="E430" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="G430" s="1" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="1" t="n">
+        <v>335</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D431" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="E431" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="G431" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="C432" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D432" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="E432" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="G432" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="1" t="n">
+        <v>337</v>
+      </c>
+      <c r="C433" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D433" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="E433" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="G433" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="C434" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="D434" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="E434" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="G434" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="D435" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="E435" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="G435" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="D436" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="E436" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="G436" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="E437" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="G437" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D438" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="E438" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="G438" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="E439" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="G439" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D440" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="E440" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="G440" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D441" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="E441" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="G441" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D442" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E442" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G442" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="1" t="n">
+        <v>347</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D443" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E443" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G443" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E444" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G444" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D445" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E445" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="G445" s="1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A446" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D446" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E446" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G446" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D447" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E447" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="G447" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D448" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E448" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G448" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D449" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E449" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G449" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A450" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D450" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E450" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G450" s="1" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D451" s="1" t="n">
+        <v>132134</v>
+      </c>
+      <c r="E451" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G451" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D452" s="1" t="n">
+        <v>732517040</v>
+      </c>
+      <c r="E452" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="G452" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D453" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E453" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G453" s="1" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D454" s="1" t="n">
+        <v>1020023</v>
+      </c>
+      <c r="E454" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G454" s="1" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D455" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E455" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G455" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D456" s="1" t="n">
+        <v>6162.0159</v>
+      </c>
+      <c r="E456" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G456" s="1" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A457" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D457" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E457" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G457" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="1" t="n">
+        <v>362</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D458" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E458" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G458" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="1" t="n">
+        <v>363</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D459" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E459" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G459" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="1" t="n">
+        <v>364</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D460" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E460" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G460" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D461" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E461" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G461" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="1" t="n">
         <v>366</v>
       </c>
-      <c r="C362" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="D362" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="E362" s="18" t="s">
-        <v>675</v>
-      </c>
-      <c r="G362" s="1" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="0" t="n">
+      <c r="C462" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D462" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E462" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G462" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="1" t="n">
         <v>367</v>
       </c>
-      <c r="C363" s="1" t="s">
-        <v>780</v>
-      </c>
-      <c r="D363" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="E363" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="G363" s="1" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D369" s="19"/>
-    </row>
-    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D370" s="19"/>
-    </row>
-    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D371" s="19"/>
-    </row>
-    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D372" s="19"/>
+      <c r="C463" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D463" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E463" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="G463" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D464" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E464" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="G464" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D465" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E465" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="G465" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D466" s="1" t="n">
+        <v>9760</v>
+      </c>
+      <c r="E466" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="G466" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D467" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E467" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="G467" s="1" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="C468" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D468" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E468" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G468" s="1" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="C469" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D469" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E469" s="1" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G469" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="C470" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D470" s="1" t="n">
+        <v>112202</v>
+      </c>
+      <c r="E470" s="1" t="s">
+        <v>1071</v>
+      </c>
+      <c r="G470" s="1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="C471" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D471" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E471" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G471" s="1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="C472" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D472" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E472" s="1" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G472" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="C473" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D473" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E473" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G473" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="C474" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D474" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E474" s="1" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G474" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="1" t="n">
+        <v>379</v>
+      </c>
+      <c r="C475" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D475" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E475" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G475" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="C476" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D476" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E476" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G476" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="1" t="n">
+        <v>381</v>
+      </c>
+      <c r="C477" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D477" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E477" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G477" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="1" t="n">
+        <v>382</v>
+      </c>
+      <c r="C478" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E478" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G478" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="1" t="n">
+        <v>383</v>
+      </c>
+      <c r="C479" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D479" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E479" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="G479" s="1" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="n">
+        <v>384</v>
+      </c>
+      <c r="C480" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D480" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E480" s="1" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G480" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D481" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E481" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G481" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="1" t="n">
+        <v>386</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D482" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E482" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="G482" s="1" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="0" t="n">
+        <v>387</v>
+      </c>
+      <c r="C483" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D483" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E483" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G483" s="1" t="s">
+        <v>1106</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I354"/>
-  <conditionalFormatting sqref="D1:D241 D243:D244 D246:D259 D261:D265 D267:D270 D272 D274:D276 D278:D279 D281:D295 E296 D297:D300 D302:D346 E347 D348:D360 D364:D1048576">
+  <conditionalFormatting sqref="D1:D241 D243:D244 D246:D259 D261:D265 D267:D270 D272 D274:D276 D278:D279 D281:D295 E296 D297:D300 D302:D346 E347 D348:D360 D364:D365 D367:D372 D374:D375 D377:D384 D386:D395 D399:D404 D408:D409 D411:D423 D425:D431 D433 D435:D1048576">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D369:D372">
+  <conditionalFormatting sqref="D369:D371">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>